<commit_message>
creates number sources table and metadata
</commit_message>
<xml_diff>
--- a/metadata/five-year-outlook-metadata.xlsx
+++ b/metadata/five-year-outlook-metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashleyvizek/code/urban-water-drought-data/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{84AE45CE-D814-AF41-B0AB-D8172179D51C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{194A4A9B-6F68-8041-80FB-986D8637B513}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29620" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29400" yWindow="1460" windowWidth="29260" windowHeight="27060" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="9" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -74,6 +74,39 @@
   </si>
   <si>
     <t>attribute_name</t>
+  </si>
+  <si>
+    <t>org_id</t>
+  </si>
+  <si>
+    <t>pwsid</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>acre_feet</t>
+  </si>
+  <si>
+    <t>DWR assigned ID number associated with the urban retail water supplier</t>
+  </si>
+  <si>
+    <t>nominal</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>ID number associated with water system in the supplier service area</t>
+  </si>
+  <si>
+    <t>is_shortage_action_included</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The volume of water (acre feet) calculated by subtracting total use from the total supply. When the "is_shortage_action_included" is FALSE this represents the water surplus or shortage when no action is applied. When the "is_shortage_action_included" is TRUE this represents the water surplus or shortage when a shortage action (either supply augmentation or demand reduction) is applied. </t>
+  </si>
+  <si>
+    <t>TRUE if shortage action is applied (includes both supply augmentation and demand reduction actions. FALSE does not include shortage actions</t>
   </si>
 </sst>
 </file>
@@ -96,18 +129,12 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -128,23 +155,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -530,22 +554,23 @@
   <dimension ref="A1:AMG10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="19.6640625" style="1"/>
-    <col min="3" max="3" width="17.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" style="1"/>
+    <col min="2" max="2" width="54.6640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="17.5" style="3" customWidth="1"/>
     <col min="4" max="4" width="13.1640625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="5.33203125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="5.6640625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="5.33203125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="5.6640625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" style="3" customWidth="1"/>
     <col min="9" max="9" width="14.1640625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="16" style="5" customWidth="1"/>
+    <col min="10" max="10" width="16" style="3" customWidth="1"/>
     <col min="11" max="11" width="17.6640625" style="3" customWidth="1"/>
-    <col min="12" max="13" width="9.1640625" style="5" customWidth="1"/>
+    <col min="12" max="13" width="9.1640625" style="3" customWidth="1"/>
     <col min="14" max="1021" width="19.6640625" style="1"/>
     <col min="1022" max="1024" width="8.33203125" customWidth="1"/>
   </cols>
@@ -554,47 +579,94 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="68" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="J2" s="4"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="7"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="5"/>
+    </row>
+    <row r="3" spans="1:13" ht="68" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="119" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="9" spans="1:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
@@ -633,19 +705,19 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.5" style="4" customWidth="1"/>
-    <col min="2" max="2" width="25.1640625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="14" style="4" customWidth="1"/>
+    <col min="1" max="1" width="20.5" style="2" customWidth="1"/>
+    <col min="2" max="2" width="25.1640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="14" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updates five year outlook table
</commit_message>
<xml_diff>
--- a/metadata/five-year-outlook-metadata.xlsx
+++ b/metadata/five-year-outlook-metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashleyvizek/code/urban-water-drought-data/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{194A4A9B-6F68-8041-80FB-986D8637B513}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7532DE0-3C24-DF45-B5B7-605BA11F142F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29400" yWindow="1460" windowWidth="29260" windowHeight="27060" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="67620" yWindow="500" windowWidth="29260" windowHeight="27060" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="9" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -85,9 +85,6 @@
     <t>year</t>
   </si>
   <si>
-    <t>acre_feet</t>
-  </si>
-  <si>
     <t>DWR assigned ID number associated with the urban retail water supplier</t>
   </si>
   <si>
@@ -100,31 +97,60 @@
     <t>ID number associated with water system in the supplier service area</t>
   </si>
   <si>
-    <t>is_shortage_action_included</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The volume of water (acre feet) calculated by subtracting total use from the total supply. When the "is_shortage_action_included" is FALSE this represents the water surplus or shortage when no action is applied. When the "is_shortage_action_included" is TRUE this represents the water surplus or shortage when a shortage action (either supply augmentation or demand reduction) is applied. </t>
-  </si>
-  <si>
-    <t>TRUE if shortage action is applied (includes both supply augmentation and demand reduction actions. FALSE does not include shortage actions</t>
+    <t>supplier_name</t>
+  </si>
+  <si>
+    <t>Name of water supplier # TODO is there a more detailed description of this</t>
+  </si>
+  <si>
+    <t># TODO how best to describe year</t>
+  </si>
+  <si>
+    <t>dateTime</t>
+  </si>
+  <si>
+    <t>YYYY</t>
+  </si>
+  <si>
+    <t>water_use_acre_feet</t>
+  </si>
+  <si>
+    <t>water_supplies_acre_feet</t>
+  </si>
+  <si>
+    <t>benefit_supply_augmentation_acre_feet</t>
+  </si>
+  <si>
+    <t>benefit_demand_reduction_acre_feet</t>
+  </si>
+  <si>
+    <t>Expected total water use (acre feet) for the given year that is assumed to be within a five-year drought period. # TODO is the assumption that total is both potable and nonpotable?</t>
+  </si>
+  <si>
+    <t>Expected total water supplies (acre feet) for the given year that is assumed to be within a five-year drought period. # TODO is the assumption that total is both potable and nonpotable?</t>
+  </si>
+  <si>
+    <t>ratio</t>
+  </si>
+  <si>
+    <t>numeric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Additional water quanity (acre feet) resulting from a supply augmentation action. </t>
+  </si>
+  <si>
+    <t>Additional water quanity (acre feet) resulting from a demand reduction action.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -155,20 +181,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -551,26 +572,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:AMG10"/>
+  <dimension ref="A1:AMG9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.6640625" style="1"/>
-    <col min="2" max="2" width="54.6640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="17.5" style="3" customWidth="1"/>
-    <col min="4" max="4" width="13.1640625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="5.33203125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="5.6640625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="14.1640625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="16" style="3" customWidth="1"/>
-    <col min="11" max="11" width="17.6640625" style="3" customWidth="1"/>
-    <col min="12" max="13" width="9.1640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="54.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="5.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="5.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.1640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="16" style="1" customWidth="1"/>
+    <col min="11" max="11" width="17.6640625" style="1" customWidth="1"/>
+    <col min="12" max="13" width="9.1640625" style="1" customWidth="1"/>
     <col min="14" max="1021" width="19.6640625" style="1"/>
     <col min="1022" max="1024" width="8.33203125" customWidth="1"/>
   </cols>
@@ -579,114 +600,197 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="68" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="E2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="5"/>
-    </row>
-    <row r="3" spans="1:13" ht="68" x14ac:dyDescent="0.2">
+      <c r="J2"/>
+      <c r="K2"/>
+      <c r="L2" s="3"/>
+    </row>
+    <row r="3" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="B4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+    </row>
+    <row r="5" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" ht="51" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" ht="119" x14ac:dyDescent="0.2">
+      <c r="E5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L5" s="1">
+        <v>2021</v>
+      </c>
+      <c r="M5" s="1">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="G10" s="6"/>
+        <v>32</v>
+      </c>
+      <c r="L6" s="1">
+        <v>10.004</v>
+      </c>
+      <c r="M6" s="1">
+        <v>1724349</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L7" s="1">
+        <v>138</v>
+      </c>
+      <c r="M7" s="1">
+        <v>2708222</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L8" s="1">
+        <v>0</v>
+      </c>
+      <c r="M8" s="1">
+        <v>432000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L9" s="1">
+        <v>0</v>
+      </c>
+      <c r="M9" s="1">
+        <v>151124</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1021" xr:uid="{00000000-0002-0000-0800-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C6 C10:C1020" xr:uid="{00000000-0002-0000-0800-000000000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1021" xr:uid="{00000000-0002-0000-0800-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E6 E10:E1020" xr:uid="{00000000-0002-0000-0800-000001000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1021" xr:uid="{00000000-0002-0000-0800-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F6 F9:F1020" xr:uid="{00000000-0002-0000-0800-000003000000}">
       <formula1>"ratio,interval"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576" xr:uid="{0E975802-AAEB-481A-9F6C-1EEB8BBDECAC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H6 H9:H1048576" xr:uid="{0E975802-AAEB-481A-9F6C-1EEB8BBDECAC}">
       <formula1>"natural,whole,integer,real"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>